<commit_message>
Benerin init lagi, nambahin add animal, cek komentar cage.cpp
</commit_message>
<xml_diff>
--- a/animal.xlsx
+++ b/animal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Literal Zoo\babi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\OOP\Tubes 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Ayam</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>food_weight</t>
+  </si>
+  <si>
+    <t>Ganti aja ya wkwkwkwk</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,6 +597,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -757,8 +766,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -804,17 +814,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1101,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,12 +1157,15 @@
       <c r="F2">
         <v>2</v>
       </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -1175,6 +1178,9 @@
         <v>55</v>
       </c>
       <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
@@ -1182,7 +1188,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -1195,6 +1201,9 @@
         <v>56</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
@@ -1202,7 +1211,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
@@ -1215,6 +1224,9 @@
         <v>57</v>
       </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
@@ -1222,7 +1234,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
@@ -1236,6 +1248,9 @@
       </c>
       <c r="F6">
         <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1257,12 +1272,15 @@
       <c r="F7">
         <v>2</v>
       </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C8" t="s">
@@ -1275,6 +1293,9 @@
         <v>60</v>
       </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
     </row>
@@ -1297,6 +1318,9 @@
       <c r="F9">
         <v>3</v>
       </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1317,6 +1341,9 @@
       <c r="F10">
         <v>2</v>
       </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1337,6 +1364,9 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11">
+        <v>1000</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1357,6 +1387,9 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1377,6 +1410,9 @@
       <c r="F13">
         <v>1</v>
       </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1397,6 +1433,9 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="G14">
+        <v>500</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1417,12 +1456,15 @@
       <c r="F15">
         <v>2</v>
       </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C16" t="s">
@@ -1437,8 +1479,11 @@
       <c r="F16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1457,8 +1502,11 @@
       <c r="F17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1477,12 +1525,15 @@
       <c r="F18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
@@ -1497,8 +1548,11 @@
       <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1517,8 +1571,11 @@
       <c r="F20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1537,8 +1594,11 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1557,8 +1617,11 @@
       <c r="F22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1577,12 +1640,15 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C24" t="s">
@@ -1596,6 +1662,15 @@
       </c>
       <c r="F24">
         <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1678,7 @@
     <sortCondition ref="D1:D23"/>
   </sortState>
   <conditionalFormatting sqref="E2:E24 F2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>